<commit_message>
Implement NE (Northeast) variant infrastructure modules
Add TWIGS-based bark ratio, crown ratio, and mortality models for the
NE variant (108 species, 13 northeastern states). NE subclasses LS models
since both use the same TWIGS equation family with different coefficients.

Key changes:
- NEBarkRatioModel: constant bark ratio per species (subclasses LSBarkRatioModel)
- NECrownRatioModel: TWIGS ACR equation (subclasses LSCrownRatioModel)
- NEMortalityModel: 4-group background mortality (subclasses LSMortalityModel)
- NE_SDI_MAXIMUMS: 108 species SDI values in StandMetricsCalculator
- 26 NE-unique species added to volume_library.py
- Fix: tree.py crown ratio update now passes variant to factory (benefits all variants)
- 38 tests passing across 9 test classes
</commit_message>
<xml_diff>
--- a/test_output/persistence_tests/yield_table.xlsx
+++ b/test_output/persistence_tests/yield_table.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,87 +422,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>tpa</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>basal_area</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>qmd</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>mean_dbh</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>top_height</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>mean_height</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>ccf</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>sdi</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>max_sdi</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>relsdi</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>volume</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>merchantable_volume</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>board_feet</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>site_index</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>initial_tpa</t>
         </is>
@@ -525,10 +513,10 @@
         <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="C2" t="n">
-        <v>0.511019023580748</v>
+        <v>0.5126185691505004</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
@@ -540,10 +528,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05675483310665119</v>
+        <v>0.05711068686699131</v>
       </c>
       <c r="H2" t="n">
-        <v>4.226798047848368</v>
+        <v>4.248052843601034</v>
       </c>
       <c r="I2" t="n">
         <v>480</v>
@@ -577,40 +565,40 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="B3" t="n">
-        <v>22.11</v>
+        <v>22.24</v>
       </c>
       <c r="C3" t="n">
-        <v>2.879129582323678</v>
+        <v>2.878962123794901</v>
       </c>
       <c r="D3" t="n">
         <v>2.88</v>
       </c>
       <c r="E3" t="n">
-        <v>22.63588915782518</v>
+        <v>22.63584059186897</v>
       </c>
       <c r="F3" t="n">
         <v>22.57</v>
       </c>
       <c r="G3" t="n">
-        <v>1.761935450383476</v>
+        <v>1.772538660352875</v>
       </c>
       <c r="H3" t="n">
-        <v>66.28619713392969</v>
+        <v>66.68663515389257</v>
       </c>
       <c r="I3" t="n">
         <v>480</v>
       </c>
       <c r="J3" t="n">
-        <v>1.380962440290202</v>
+        <v>1.389304899039429</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
       </c>
       <c r="L3" t="n">
-        <v>319.93</v>
+        <v>321.86</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -632,40 +620,40 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B4" t="n">
-        <v>53.6</v>
+        <v>50.19</v>
       </c>
       <c r="C4" t="n">
-        <v>4.519986719273934</v>
+        <v>4.360260466518791</v>
       </c>
       <c r="D4" t="n">
-        <v>4.52</v>
+        <v>4.36</v>
       </c>
       <c r="E4" t="n">
-        <v>36.09334023314045</v>
+        <v>36.0926112263078</v>
       </c>
       <c r="F4" t="n">
-        <v>36.03</v>
+        <v>36.02</v>
       </c>
       <c r="G4" t="n">
-        <v>2.953300250376031</v>
+        <v>2.847068023443553</v>
       </c>
       <c r="H4" t="n">
-        <v>134.4745860826723</v>
+        <v>127.7211490456516</v>
       </c>
       <c r="I4" t="n">
         <v>480</v>
       </c>
       <c r="J4" t="n">
-        <v>2.801553876722341</v>
+        <v>2.660857271784409</v>
       </c>
       <c r="K4" t="n">
         <v>10</v>
       </c>
       <c r="L4" t="n">
-        <v>974.9</v>
+        <v>918.85</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Bump version to 0.3.0 and update project description and README
Update pyproject.toml description, keywords, and classifiers to reflect
10 regional variants, taper-based volume system, and 500+ species configs.
Rewrite README with multi-variant examples, volume system docs, architecture
overview, and variant-specific growth equation comparison table. Update
__init__.py docstring and version. Include regenerated test outputs from
taper volume integration and untracked variant config files.
</commit_message>
<xml_diff>
--- a/test_output/persistence_tests/yield_table.xlsx
+++ b/test_output/persistence_tests/yield_table.xlsx
@@ -513,10 +513,10 @@
         <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5126185691505004</v>
+        <v>0.5091693569921298</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
@@ -528,10 +528,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05711068686699131</v>
+        <v>0.05634472104730723</v>
       </c>
       <c r="H2" t="n">
-        <v>4.248052843601034</v>
+        <v>4.202269778071582</v>
       </c>
       <c r="I2" t="n">
         <v>480</v>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>93.62</v>
+        <v>93.61</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -565,40 +565,40 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B3" t="n">
-        <v>22.24</v>
+        <v>22.29</v>
       </c>
       <c r="C3" t="n">
-        <v>2.878962123794901</v>
+        <v>2.879256230121726</v>
       </c>
       <c r="D3" t="n">
         <v>2.88</v>
       </c>
       <c r="E3" t="n">
-        <v>22.63584059186897</v>
+        <v>22.63594512880691</v>
       </c>
       <c r="F3" t="n">
         <v>22.57</v>
       </c>
       <c r="G3" t="n">
-        <v>1.772538660352875</v>
+        <v>1.776504290531661</v>
       </c>
       <c r="H3" t="n">
-        <v>66.68663515389257</v>
+        <v>66.83313373782879</v>
       </c>
       <c r="I3" t="n">
         <v>480</v>
       </c>
       <c r="J3" t="n">
-        <v>1.389304899039429</v>
+        <v>1.392356952871433</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
       </c>
       <c r="L3" t="n">
-        <v>321.86</v>
+        <v>169.53</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -620,40 +620,40 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B4" t="n">
-        <v>50.19</v>
+        <v>49.87</v>
       </c>
       <c r="C4" t="n">
-        <v>4.360260466518791</v>
+        <v>4.35991106436567</v>
       </c>
       <c r="D4" t="n">
         <v>4.36</v>
       </c>
       <c r="E4" t="n">
-        <v>36.0926112263078</v>
+        <v>36.09245303066545</v>
       </c>
       <c r="F4" t="n">
         <v>36.02</v>
       </c>
       <c r="G4" t="n">
-        <v>2.847068023443553</v>
+        <v>2.829153345215149</v>
       </c>
       <c r="H4" t="n">
-        <v>127.7211490456516</v>
+        <v>126.9131645197708</v>
       </c>
       <c r="I4" t="n">
         <v>480</v>
       </c>
       <c r="J4" t="n">
-        <v>2.660857271784409</v>
+        <v>2.644024260828557</v>
       </c>
       <c r="K4" t="n">
         <v>10</v>
       </c>
       <c r="L4" t="n">
-        <v>918.85</v>
+        <v>694.28</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>

</xml_diff>